<commit_message>
Get daily reddit data: Tue Aug  6 08:09:42 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_08_11.xlsx
+++ b/data/2024_08_11.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C472"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5551,6 +5551,2914 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1elbt2u</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>I did these my self they r just extentions and gel effect polish how good r they(im 13 btw)</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1elbt2u</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1el7usk</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t xml:space="preserve">White on white French. </t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gjomuo1ssygd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1ela2yb</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>Quality gel polish brands available in Australia?</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ela2yb/quality_gel_polish_brands_available_in_australia/</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1el9oo6</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My first set on myself </t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1el9oo6</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1el8l84</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tried press ons for the first time! </t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0auuqgjxzygd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1elahzb</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>Got my nails done because I’m ENGAGED! 😍💅🏼💍</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1elahzb</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1ela22z</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>Did my own Gel nails for first time! What do you think?</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7ahvdvkrfzgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1ela1u2</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail art with clear polish? </t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ela1u2/nail_art_with_clear_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1el9jla</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What do you think of the change? </t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1el9jla</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1el99bf</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>Men can wear nails too!</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1el99bf</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1el90ys</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>Ice Truck Killer nails from Dexter in honor of the upcoming prequel!</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ou1jhd1c3zgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1el90jr</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail dump 💫 hard gel structured manicures on all my client’s natural lengths </t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1el90jr</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1el8wo5</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>Ombre nails, what do you think?</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oo0qce783zgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1el8u1e</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>one of my fav press ons🥰</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xr6939df2zgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1el8n72</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>Male pedi question</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1el8n72/male_pedi_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1el8jj6</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>Color changing!</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1el8jj6</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1el7oyz</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I did something different and I’m super happy! Can’t stop staring at them. </t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/lzzo3fz8rygd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1el7lc1</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail salon said they will fix for free, nervous incase it looks like nothing should I fix or leave ? </t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/le4xfrxbqygd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1el6mid</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cinderella Blue 👸 </t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o33dlfekhygd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1el5fbe</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>Marble short</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1el5fbe</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1ekzqca</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>Help?! Cuticle &amp; Nail Skin</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ekzqca</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1el5ekt</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>Cuticle help</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sf4wegaw6ygd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1el6bpe</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>Tip isn't flush with my natural nail. Should it be redone?</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1el6bpe</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1el6ayn</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t xml:space="preserve">So juicy 😋 What do you guys think of these summer sets I did?! 😍 I’m could eat them all up. </t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1el6ayn</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1el64ru</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>How do they look and how can I improve?</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1el64ru</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1el5xy4</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>Fake “natural nails”</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1el5xy4</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1el5qxx</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dark Mermaid Press Ons I made. </t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1el5qxx</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1el5j38</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Yay or nay? How much would you pay for these? </t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w1n2nbzy7ygd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1el5hby</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>First ever painting of my nails 30M Chemical X</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ebyf02gj7ygd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1el59jd</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>green and gray 💚🩶</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1el59jd</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1el50n7</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>Do these look like press-ons?</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1el50n7</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1el50bv</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>🩷🍓Favorite Set Ever!🍓🩷</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1el50bv</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1el4w1i</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>Gel X nails!</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1el4w1i</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1el4r9c</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>Just a black nail girlie. 🖤</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8bqs09gf1ygd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1el4qi4</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Turtle nails! </t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1el4qi4</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1el4ndb</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>Letting My Nails Grow: Week 9</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qhuxatxh0ygd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1el4bkc</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>Sea glass nails. I loved doing these</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1el4bkc</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1el3thp</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Adding another layer of gel top coat </t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1el3thp/adding_another_layer_of_gel_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1el3lyg</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>When your nails match your scrubs</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wjo2wv9wrxgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1el3j9o</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>Press ons or nail salon?</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/prdljgwarxgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1el3fc2</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>I once again did my boyfriends nails, this time Naruto themed (his favorite show)</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1el3fc2</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1el2ur6</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>I fear I undercharged,  curious what you’d pay for set🐚🫧⭐️</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kcu9s9mulxgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1el2l7w</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>Press-ons + stickers! How good do they look?</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lxcpmwzpjxgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1el2kt5</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Treated myself and I’m obsessed </t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o7ubftgkjxgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1el222w</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>What color should I choose?</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1el222w</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1el1c7r</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>What shape are my natural nails?</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xp0l9yw5axgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1el1ea8</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>Kiss press ons</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1el1ea8</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1el0ga0</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tried nail art for the first time. This was the best I could do. </t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c44x5xun3xgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1el06jg</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>Opinions on MakarttPro?</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l7l4zgxl1xgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1el064r</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>Pretty impressed with these press ons</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1el064r</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1ekzkbe</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>F1 Nail Art!!</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ekzkbe</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1ekzhum</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cadillaquer - Reflections </t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ot5yfk6owwgd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1ekytla</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>Can I just use cuticle remover instead of an e-file for the cuticle?</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ekytla/can_i_just_use_cuticle_remover_instead_of_an/</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1ekze86</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>HELP</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rgbx3u1yvwgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1ekzape</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>What do you think of this angelic design? 🌸🪽</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nacahw09vwgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1ekypiv</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>My Nocturnal Wonderland 2024 Nails</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9q8n3h81rwgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1ekz42l</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sparkle ✨️ </t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a41l3ymwtwgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1ekyvc6</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>Cute</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7stl3gg7swgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1eky55s</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>Sally sells seashells by the seashore. 🌊🐚</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uxvpncd1nwgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1ekxti3</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>My hand and nails, natural...!!!</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ekxti3</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1ekxnkg</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>Experimented with new gellac for the first time - Proud moment</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5yok30ajjwgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1ekxlm9</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>How to file/shape my nails to strengthen them?</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ekxlm9</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1ekxh8y</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>Ex Nail Biter: Nail Shape and Filing Suggestions?</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ekxh8y</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1ekxeyw</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Wanted chrome. This isn't it. </t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vjwlxaxuhwgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1ekxef1</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>So happy with my nails!</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ekxef1</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1ekxbkw</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>Perks of being your own nail tech: You can SHAMELESSLY let the impulsive urges on a random Sunday afternoon take over 😌💅</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ekxbkw</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1ekx7qe</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>Do these look real or like press-ons?</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ekx7qe</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1ekwk7b</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>Help! Middle of my nails are turning brown from builder gel</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ekwk7b/help_middle_of_my_nails_are_turning_brown_from/</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1ekw7fn</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>I got over my fear of the nail salon!</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qbmejf699wgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1ekwzva</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>I would love a honest opinion</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ekwzva</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1ekw1vd</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t xml:space="preserve">For $5?!? Can't beat it </t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4zc2y0s58wgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1ekv1vx</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>Nails</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ekv1vx</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1ekusav</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>Seashell 🐚</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7dobkvz6zvgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1ekuoqa</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>Need Validation !😆</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ekuoqa</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1ekulxf</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>Black cherry 🍒</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ekulxf</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1ekulsq</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>My wedding set, got them done at a nail salon</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ekulsq</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1ekuf9g</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>Does it look too press on-y?</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qckk3w7pwvgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1ekud0v</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Need ideas for vacation! </t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ekud0v/need_ideas_for_vacation/</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1ektyzk</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hi everyone! New here! </t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xdal1u2gtvgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1ektq24</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>Structure Gel or Gel X</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ektq24/structure_gel_or_gel_x/</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1ektfgx</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What do you think? </t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ektfgx</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1ektdp7</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>Very new to nail art😅</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nxm90j97pvgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1ekhchi</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>WHAT'S WRONG WITH MY NAILS</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ekhchi</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1ekt4ng</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t xml:space="preserve">my first longg set. opinions? </t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2hgimlnfnvgd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1eksrrz</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>Builders Gel for Half Toenail</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eksrrz/builders_gel_for_half_toenail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1ekstjy</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Did my sisters nails beach themed because shes going on vacation! </t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ekstjy</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1eks2ga</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>Nail tech didn’t give me chrome powder</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eks2ga/nail_tech_didnt_give_me_chrome_powder/</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1eksc0i</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>Low rider inspired set ❤️</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eksc0i</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1ekryhf</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>Paris Nails</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1a35q2e0fvgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1ekrhtr</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>Chrome and Magnetic Fun</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ekrhtr</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1ekqtia</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Builder gel </t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ekqtia</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1eki40x</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>need advise to improve my nails and cuticles</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eki40x</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1ekqwbt</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>How do these look?</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ekqwbt</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1ekqq7c</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>Painted my nails, I don’t think they’re that bad!</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n7jt0ab86vgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1eki69u</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>Good Korean gel polish brands?</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eki69u/good_korean_gel_polish_brands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1ekm1x1</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>Question. First time ever getting long nails</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ekm1x1/question_first_time_ever_getting_long_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1ekqfbs</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>Cherry Red Nails 🍒</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tlivi2044vgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1ekqe15</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>i foundsome old acrylics. notmade for me but thought it would be fun sticking it on. howd i do?(icant type help)</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ekqe15</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1ekp6p5</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>Reusing press on nails?</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ekp6p5/reusing_press_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1ekq9gi</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>Was going for jelly nails but derailed midway lol</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ekq9gi</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1ela1zy</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Vacation shimmer ✨ </t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/261x5t0rfzgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1el87i4</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>I'd rather stay up looking my nails</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/sh6b69y6wygd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1el6ojq</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>Neutral, but not boring 🤩</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1el6ojq</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1el6kb8</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>First time stamping!</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1el6kb8</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1el5wr0</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>Everything but the Kitchen Sink - Restored by Polish</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1el5wr0</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1el48dq</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>i feel like i have jewels on my nails</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1el48dq</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1el3r5m</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>Fairy nails 🧚</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1el3r5m</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1el3c92</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>Help! Going bowling, how do I protect my nails?</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1el3c92/help_going_bowling_how_do_i_protect_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1el2oww</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>Mooncat “Hardcore Buttercup” and “Chemical X” (over 1 coat of black)</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1el2oww</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1el1ns7</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>Excuse Me While I Kiss This Guy | Mermaid Bait</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1el1ns7</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1el18x1</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time nail art </t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1el18x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1el0r7y</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>Maybe went a little crazy</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/twjiosyv5xgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1el05x7</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is anyone else too lazy to do nail art most of the time? I really should get out my stamping stuff more often. </t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ffh6tomh1xgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1el03ix</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>Post partum nails</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1el03ix/post_partum_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1el02xr</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>Death Valley Nails! (long post + some experiments!)</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1el02xr</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1ekksgr</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>Neutral everyday nails</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ojio1d9ustgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1ekzm24</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>Cadillaquer-Reflections</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ekzm24</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1ekyp4a</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>Spanish tile vibes!</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fn6f1hnuqwgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1eky6la</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>Feeling very witchy. Samhain by Dany Vianna</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eky6la</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1ek9x7q</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>Dupe for Circus Chic by DND</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ek9x7q/dupe_for_circus_chic_by_dnd/</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1ekwu40</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>(PR) Evil eye nails 🧿✨</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3br1cr4pdwgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1ekwk18</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>Swamp gloss - But Elijah Wood</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ekwk18</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1ekwix6</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>Tectonic Shift</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ekwix6</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1ekux5x</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>BKL The Foxglove King relatives?</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ekux5x/bkl_the_foxglove_king_relatives/</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1ekulx0</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>I slept on this shade for too long</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ekulx0</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1ekuh2y</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>Can Bis-HEMA cause an allergy?</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z263p072xvgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1eku9dn</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>25 Fly</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eku9dn</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1eku0bj</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Feeling foxy wearing Nickit </t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eku0bj</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1ektqk6</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Verdigris vs. Brace For The Fallout
+</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ektqk6</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1eksv4l</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>Getting back into nail art</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eksv4l</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1eksoih</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>My current mani: desaturated Summer skittle🩶</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eksoih</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1ekshzp</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>I am a donut</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bk5or6dxivgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1eks7zy</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t xml:space="preserve">GelX second application! Loving this product! </t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eks7zy</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1eks3ux</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>Paco's Nails in Paris (Happy Checkmate)</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m0puzby0gvgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1eks28p</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>How do I go about sanitising the brush part of my oil pen without damaging it/making it flare out?</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cpd2vyulfvgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1ekrzw7</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>Butterfly Wings!</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ekrzw7</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1ekra98</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Xu Xialing and Shang-Chi nails </t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1cuyjieaavgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1ekr6pd</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>Lighthouse Nails!</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ekr6pd</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1ekpvna</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>Out of this world mani 🛸👽</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ekpvna</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1ekp56r</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can anyone identify this KBShimmer? </t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ekp56r</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1eko4m6</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t xml:space="preserve">China Glaze is rebranding and there will not be a 2024 Summer, Fall, or Winter collection. Watch Janixa from NailLacquerTherapy’s video for more details! I’m curious if this means they will discontinue some of their existing core colors and what this means for Salon Perfect (which is owned by CG) </t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://youtu.be/mnql8pa40IE?si=96cCHpnIgl6IluU3</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1ekn72t</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ethereal Lacquer Matcha Cloud </t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ekn72t</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1ekmi8i</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>DS Lite cover dupe?</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fuui5exw9ugd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1ekmdxl</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>Bling and Blowing Bubbles</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ekmdxl</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1ekl8dm</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>Help picking a design?</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ywmu9c6lxtgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1ekkklg</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>So what color is this? Any ideas for dupes?</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u1gn9py49ogd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1ekjzxj</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ekjzxj/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1ek2ngl</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Please advice me on nailpolish brand </t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ek2ngl/please_advice_me_on_nailpolish_brand/</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1elbnlx</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>tell me your thoughts 🤔</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jpexk4s9yzgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1elbe3w</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t xml:space="preserve">August nails </t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m5f29auxuzgd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1elb70w</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>who doesn’t like coffee right</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mq400g2sszgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1elb677</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>My design inspired by Astarion from Baldur's Gate 3 💅</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1elb677</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1el9km3</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>What my client wanted VS what she got 🥹</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1el9km3</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1el9igs</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t xml:space="preserve">DUCKIEZZ😍 I’m obsessed with my 3D doll!! </t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1el9igs</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1el7yyo</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>HOW CUTE 🎀</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vfwlsdvutygd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1el6ypw</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>Took some trial and error…</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1el6ypw</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1el1vmq</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>Sea glass nails 💅 I’m in love</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1el1vmq</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1el1rhc</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>Witchy dark vibes 🐍🖤</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1el1rhc</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1el0kfu</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>More press ons :D was given these heart charms and I just had to do something with them</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1el0kfu</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1el0hc7</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>Fresh set - O Nail Spa, Ellen</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s5c27o7a3xgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1ekz8m8</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>My 3 month nail journey so far :)</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ekz8m8</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1ekybvt</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>Loving this set.</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y66y015cowgd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1ekybrg</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>What and where to get good polish</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1ekybrg/what_and_where_to_get_good_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1ekxouj</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Close ups (gothic black &amp; red nails) </t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ekxouj</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1ekwqmd</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Red &amp; black gothic nails </t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ekwqmd</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1ekwb1j</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> I try this idea do you like it</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/qqmz2nyi9wgd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1ekuzw5</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>love my nails!!</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1sulzmlp0wgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1ekutcn</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>Jade Jewels 💚🐲</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sv1uvqqezvgd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1eksqlu</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Press on set I did on myself </t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eksqlu</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1ekrjph</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>rate this set</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ekrjph</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1ekovhu</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>A beautiful butterfly and a flower. What do you think?</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tffk3btysugd1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Aug  7 08:09:40 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_08_11.xlsx
+++ b/data/2024_08_11.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C472"/>
+  <dimension ref="A1:C634"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8459,6 +8459,2760 @@
         </is>
       </c>
     </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1em5uyq</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>First time</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/suivdlns47hd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1em5irv</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>Tried to do a firework accent nail</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1em5irv</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1em3kov</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>I think I have enough… :D</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1em3kov</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1em3dji</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t xml:space="preserve">😍Frenchies </t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jyjfhc37c6hd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1em2d3n</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Brush broken </t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ss1osilz16hd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1em34ga</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>Stupid Question?</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1em34ga/stupid_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1em33t4</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>i love doing my own nails!!</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1em33t4</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1em2zsk</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>My nubby nails before and after😰</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1em2zsk</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1em2wfg</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>Advice for best nail products for someone who doesn't like having their nails done?</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/czq694ia76hd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1em1vk4</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>hard gel american mani on me by me :)</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ucokhccx5hd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1em1jse</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>rate my new lilac pressons🦋🪻</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1em1jse</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1em141q</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>Design thoughts??</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1em141q</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1em140f</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t xml:space="preserve">new set!! </t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r4kgkwifq5hd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1em0q5q</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t xml:space="preserve">40th Birthday (almost) Nails! </t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1em0q5q</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1em0nas</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>First time doing almond nails with IBD Builder Gel!</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1em0nas</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1em0m8u</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>Duckiezzz🥰</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1em0m8u</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1elym4j</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>the vibes are immaculate✨🖤🧚🏼‍♀️</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1elym4j</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1elztsl</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>Would you wear these nails?! Gothic freestyle for my beautiful client ☠️😮‍💨🥰</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1elztsl</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1elzm5n</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>Butchered my nails from efiling for the first time 😂 tips on how to heal them faster?</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r94i46pad5hd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1em0c22</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>First short nail mani!</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1em0c22</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1em0ade</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>Did I tip too much?</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9w7folk3j5hd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1elzbjb</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>Elopement Nails ✨🖤</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qnib625ra5hd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1elzadb</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My favorite nails of all time </t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/frp5ecfga5hd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1elz814</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>dispose of nail glue?</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1elz814/dispose_of_nail_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1elz4st</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>Did my own nails for my wedding! 💍</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/irswoby595hd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1elyur8</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MOTHMAN </t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4p4wex8t65hd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1elyij7</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>I feel like I have tiny tuxedos on my hands 😆🤵🏼‍♀️</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l2nsn8i045hd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1ely9em</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>{PR} Sassy Sauce | Polish Pick Up | Wet Spot</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ely9em</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1ely6op</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>Urge to cut nails short?</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ely6op/urge_to_cut_nails_short/</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1ely0n2</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>First time without nail extensions in a long time, it feels so bizarre!! DIY</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n9b8qjfkz4hd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1elxydd</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Covid was great for keeping my hands out of my mouth. Natural nails </t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3y77e1acz4hd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1elxwax</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I want to start teaching myself gel mani. Can you link me to good quality products I’ll need? Maybe some good YouTube links too? I’d like to have nice nails and not break my bank </t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1elxwax/i_want_to_start_teaching_myself_gel_mani_can_you/</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1elxvcn</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>I’m obsessed 💜</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/of77o8bny4hd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1elxqsn</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>Just want to show you my nails 😄</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nymutf4lx4hd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1elxevh</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>What do you think of this design? I made it myself ☺️</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0rzfrt4xu4hd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1elxe5v</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>A modern and fresh French for the occasion</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a1uthc3ru4hd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1elx0r8</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>Bday ideas!</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1elx0r8/bday_ideas/</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1elw06h</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>Same design different shape. Which one does it suit more</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1elw06h</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1elwbke</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Rubber base doesn't cure rock hard? </t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1elwbke/rubber_base_doesnt_cure_rock_hard/</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1elwp4e</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>And here my niece is learning to do nails 💙 I loved them, what do you think? 💅💙</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1elwp4e</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1elwgj1</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>🌻💅🏼 my favorite set</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1sa58e67n4hd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1elvxht</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>First set of my own press ons! Plus a question about fit</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1elvxht</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1elvuc6</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>which shape do you prefer on me?</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1elvuc6</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1elu19s</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>First time ever using gel polish. Thoughts? I bought red/maroon polish but the wrong colour showed up :(</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1elu19s</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1elvd1c</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>What are these strange bubbles? How do I fix them?</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://reddit-uploaded-media.s3-accelerate.amazonaws.com/f0ubatmte4hd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1elvn3s</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>starry night inspired</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1elvn3s</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1elvo60</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>The prettiest set Ive ever gotten!</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qbgcdyd9h4hd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1elvnx3</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>Please tell me if my nail lools good. I did them myself</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wa6oabg5h4hd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1elvg5o</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Last months nails </t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1elvg5o</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1elv63h</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>new nails 🫶</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2e9bs3oed4hd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1elv5w5</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t xml:space="preserve">basic but i love this color </t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0qmrr12dd4hd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1elur70</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>Accidentally matched my polish to my living room 🤷🏽‍♀️</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1elur70</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1elucjn</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>Summer floral Nails 🌺🌼</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d1ic1xyc74hd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1eltyg3</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How should nails look from the side? </t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eltyg3</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1eltugh</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>Looking for Pre-Wedding Nail Salon with Wine/Champagne in CT</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eltugh/looking_for_prewedding_nail_salon_with/</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1eltite</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I’d like to thank god and baby hormones </t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eltite</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1elsh7t</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>Luxio equivalent of OPI’s funny bunny?</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1elsh7t/luxio_equivalent_of_opis_funny_bunny/</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1elswar</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>Opinions? I did them myself (I know they are a bit bumpy)</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d38107sww3hd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1elrsd9</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t xml:space="preserve">just got these done 💅🏻 </t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2f3v3w55p3hd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1elrhm8</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>Simple bling 😁</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xc2y7031n3hd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1elr3p5</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t xml:space="preserve">these are the cutest set of nails I've ever had I could scream! </t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1elr3p5</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1elqss5</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>Is it ever too early for Halloween nails?</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qcy84adyh3hd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1elpz2c</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>First time using press-ons</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v84v8du1c3hd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1elnt9x</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>What do we think of my nails?</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hth7o3gww2hd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1elnhvm</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>Absolutely in love with how this turned out for 😍</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1elnhvm</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1elmuii</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>Cracked nail treatment???</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1elmuii/cracked_nail_treatment/</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1elauu5</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>Can someone help?</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1elauu5</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1eln9am</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Good match for skin tone </t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lx652b4vs2hd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1eln2c7</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>Black gel 🖤</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eln2c7</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1elmpoa</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>Slowly branching out…a little bit, with colored tips.</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1elmpoa</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1elmljh</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I heard matte was in... What u think? </t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1elmljh</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1elmkoq</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>Press-ons both hands :)</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1elmkoq/pressons_both_hands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1elmgw4</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>French and classic style</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kz74btaan2hd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1elmcmk</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Need some help </t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1elmcmk</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1elmeah</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>Better pics of my nails I did</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1elmeah</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1elm6s8</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>Best nail shapes for those who bite</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1elm6s8/best_nail_shapes_for_those_who_bite/</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1ellut8</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>I loved the combination of blue and silver.</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o02neioyi2hd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1ells82</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Looking for opinions </t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ells82</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1elazab</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>Peeling nails fixed… what next!</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1elazab/peeling_nails_fixed_what_next/</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1elbnn1</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>Gel polish discoloration/stain</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1elbnn1</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1elcc1c</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>Nail colour for hope/positive vibes</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1elcc1c/nail_colour_for_hopepositive_vibes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1elggqb</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>BEST matte top coat for chrome?!</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1elggqb/best_matte_top_coat_for_chrome/</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1elgz5h</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>Fake Nails Questions (Flat nail peeps?)</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1elgz5h/fake_nails_questions_flat_nail_peeps/</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1eljsrg</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>Press ons</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d0yx0fog42hd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1elli7l</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>What do you think of this design? They like?</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3g8sxdukg2hd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1ellcxw</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>Suggestions to improve?</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ellcxw</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1ell3by</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>Just did my nails, do you like them?</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lm63igbmd2hd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1elkrll</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>I think i've been cutting my nails wrong all my life?</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rnp0vf38b2hd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1elkpzh</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>I got new nails done.</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7un9dj7za2hd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1elkg4g</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t xml:space="preserve">double french tip mani! </t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1elkg4g</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1elkdsb</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>Freshly done nails</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1elkdsb</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1elk2ng</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Did them myself... What do you think? </t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/396894ef62hd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1eljurb</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>little swirly nail action 🤍</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o8cjpmpu42hd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1elip63</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>Strawberry Jelly Nails</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y757dz5gw1hd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1elioyw</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>Finally a set I did on myself that I actually like lol</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1elioyw</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1eli20o</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>My first attempt to do my own nails (half cured gel). What do you think?</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rp7bvqflr1hd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1elhraq</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>Update: used a pinker nude</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u67qqz98p1hd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1elh732</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>💍 Need Your Help: Nail Color for Sapphire Engagement Ring 💅</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1elh732/need_your_help_nail_color_for_sapphire_engagement/</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1elgg8k</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>Just got those lovelies done, what do we think?</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wxqu3tkle1hd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1elgc2c</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Not sure if my nails look nice but i find this shot very aesthetic </t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vw6kqimrd1hd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1em63ty</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>Nail Glue as Sealant</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1em63ty/nail_glue_as_sealant/</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1em61z3</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>is it giving brat? shrek? duolingo???</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1em61z3</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1em5j1v</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>UPDATE: Seeking Baby Pink Lacquer</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g0rkrbtr07hd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1em50r1</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>INM Out the door</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1em50r1/inm_out_the_door/</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1em380e</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>The Watery really is watery</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1em380e</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1em329d</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>3d nail art?</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1em329d/3d_nail_art/</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1em23sb</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>Goopy top coat</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qq1ipz5iz5hd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1em1ku7</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>Paranoid of gel allergy, but can I use my gel polished to make press-ons?</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1em1ku7/paranoid_of_gel_allergy_but_can_i_use_my_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1em1j5n</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>Don’t Tell Vintage_Dusties</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gr1wn575u5hd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1em15pa</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dreamland lacquer— Shake your Shamrock </t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1em15pa</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1em0qmn</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Embracing my inner gremlin with a good ol’ prugly </t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9dg1ffw4n5hd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1em0q7f</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>Burgundy Creme 🍒</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/6-8-2024-xDaZACG</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1elzjmh</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Starrily Silent Night Sky over black 🖤 </t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/quswgq3oc5hd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1elzigv</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>The Skittle That Was Promised (LynB)</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1elzigv</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1elzhb7</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I grabbed this as soon as the BKL store opened in June. Saved the package for a rainy day. A tropical storm just came through so it felt right to pull it out. </t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1elzhb7</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1elyvhv</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>Decided it was time for a palette cleanser, so I did a sheer sort of pearly champagne shimmer 🍾💫</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1elyvhv</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1elyksf</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>Stamping plus ombre!</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1elyksf</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1elyb6w</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>{PR} Sassy Sauce | Polish Pick Up | Wet Spot</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/kdy7q2fa25hd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1elwlxf</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>Garden Path Lacquers Contentment</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1elwlxf</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1elwkeh</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>Garden of Evil is gorgeous 🥰</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1elwkeh</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1elvhjo</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Last months nails </t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1elvhjo</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1elv34e</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>Love looking at my nails in this lighting!</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1elv34e</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1eluvxl</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>Orly Passion Fruit topped with kbshimmer Frequent Flyer (and seche vite)</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5m6e8n9cb4hd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1elufrz</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>ILNP Flower Child on my shorties 💖</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1elufrz</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1eluaf1</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>Atomic Polish Sour Apple Rings</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/m7rzoaux64hd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1elu27u</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>“Glass Swan”</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1elu27u</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1eltfxs</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>How are we fixing hangnails these days?</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/24w8kils04hd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1elsnzs</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Am I crazy or does this polish make my nails look dirty?? </t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1elsnzs</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1elsbm8</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>geometric french tips</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1elsbm8</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1elrzsp</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>Has anyone ordered from Crystal Knockout?</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1elrzsp/has_anyone_ordered_from_crystal_knockout/</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1elrwt9</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>Am I experiencing a gel nail allergy?</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1elrwt9/am_i_experiencing_a_gel_nail_allergy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1elrmyd</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>I am a reformed cuticle/skin fold nipper!</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1elrmyd/i_am_a_reformed_cuticleskin_fold_nipper/</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1elpvf2</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>It takes two to Tango 🍊</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1elpvf2</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1elpfzu</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>I compared Mooncat velvet rose with Cirque BAE</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1elpfzu</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1elmsl9</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Why is the holo gone? </t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1elmsl9</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1elmhxf</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>Cuticle oil for nail biters?</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1elmhxf/cuticle_oil_for_nail_biters/</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1ellusr</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>Bees Knees, Praise the Shaggy Dog 🐾</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ojro6yoxi2hd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1ellp1y</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>My nails are a Pool 🏊‍♀️</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ellp1y</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1ell9gc</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>Toe Color Suggestion Needed</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ell9gc</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1elks19</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Metallic flowers 🌸 </t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xn9uptgdb2hd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1eljwfr</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>{PR} Pink Lemonade by ILNP</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ubhf4zw852hd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1eljuhn</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>Pizza and nail polish, my faves 😍</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eljuhn</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1eljbc5</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>The hype around My Life As a Shrimp is so worth it</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/daz7clfy02hd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1elhubj</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>We need to talk about Wooly</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1elhubj</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1elha3u</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>Fall in love again and again 🍏</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/bfBZHnR</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1elgtxk</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>Best Recommended One Coaters</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1elgtxk/best_recommended_one_coaters/</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1elgjrx</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>Got my festival nails done. My lady killed it!</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/aguBZ0S</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1elexvu</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My Vision inspired nail art </t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/awhucyam01hd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1eld4ba</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>First try with polish after a while</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/of7awmr5g0hd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1elxu52</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Flower Nails </t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/znyqbkjay4hd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1elveb0</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>Character set on my client🌸</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1elveb0</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1elto9g</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>Casino Nails</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1elto9g</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1elt29o</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>LOVE 💓</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8wrhmki4y3hd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1elsgl0</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>inspired by bongs n the like</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6m5zmlkst3hd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1elrtks</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love vibrant and contrasting colors. Would you wear it on your nails? </t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b7byzq2dp3hd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1elogpm</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t xml:space="preserve">the most beautiful thing you will see today!! </t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t9nblq6i13hd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1elo0bp</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>Roja nailz❤️❤️❤️👠🎒🌹💅</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1elo0bp</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1elncfx</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>Decals have been a game changer!</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1elncfx</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1ellikb</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>basic set i did, edges are raggedy</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t3ac4ygmg2hd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1ellgz9</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>Abstract Chrome</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ellgz9</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1ellflw</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>Summer fun</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w5u6jov1g2hd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1elj8nw</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>Short black and blue ombré</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ordsr2hc02hd1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Aug  8 08:09:31 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_08_11.xlsx
+++ b/data/2024_08_11.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C634"/>
+  <dimension ref="A1:C803"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11213,6 +11213,2879 @@
         </is>
       </c>
     </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1en0cab</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>First time nail art</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1en0cab/first_time_nail_art/</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1emzo8m</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>Tips and advice for beginners.</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1emzo8m/tips_and_advice_for_beginners/</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1emzo4f</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>Abstract Chrome Design</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1emzo4f</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1emzjdi</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>cute star :3</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1emzjdi</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1emzdmo</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>I wanna do my nails</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1emzdmo/i_wanna_do_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1emvdve</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>Maybe a silly question .. but nail care</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1emvdve/maybe_a_silly_question_but_nail_care/</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1emy3qg</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>help!</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1emy3qg/help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1emykp0</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>I loved my creation today</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4a8wna71tdhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1emyhg5</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>First time getting nails done at a salon! Is this a normal nail job?</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wt0a29bwrdhd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1emyfa9</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>Nails I painted this week :&gt;</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1emyfa9</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1emy3qc</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fresh set </t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7dpz3a5pndhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1emy254</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>I am in love with this BLUE! 🤩</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0fcbuu37ndhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1emxhh2</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>Love these colors!</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6poqj7z0hdhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1emx8lt</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>My “chrome” dupe</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1emx8lt</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1emvpwv</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>inspired by seventeen</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1emvpwv</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1emw5lt</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t xml:space="preserve">new nails </t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/97nm2t8t3dhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1emx0h9</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>{PR} Sassy Sauce | Polish Pick Up - Not your Mama’s fairy tale</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1emx0h9</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1emwtto</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>Is this nail art?</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1emwtto</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1emwryk</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>Got my nails done for the first time today 💅🏽</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qjfp4spq9dhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1emwiiu</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>What do you think of these press ons?</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1emwiiu</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1emwcfa</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>My nail tech killed it today 🤩</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oqgc2dan5dhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1emw5kh</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>Does the almond shape suit me?</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xunflt4t3dhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1emvog5</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>Nail advice</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1emvog5/nail_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1emvlxn</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>Does jojoba oil leave your fingers greasy?</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1emvlxn/does_jojoba_oil_leave_your_fingers_greasy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1emvd0d</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>My nails are super flat and weak! Help</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1emvd0d/my_nails_are_super_flat_and_weak_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1emv3ga</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>These remind me of a summer sunset 🌅</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nyy55qq0uchd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1emunph</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>Reflective polish gets me every time</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t48vdfb5qchd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1emujxg</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>Gothic opal set I did on myself 🖤</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fbctyj08pchd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1emuegr</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>Traditional red nail polish</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hvgwc1iwnchd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1emue93</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>MIAMI PINK!</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1emue93</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1emuc7o</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Did my nail </t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5prsv0rcnchd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1emtzu2</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>I asked for a birthday set❣️</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ivfep1hikchd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1emts49</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>My nails need some color!!!!</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x1pym0voichd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1emtrj7</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>I love getting my nails done 🩷</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1emtrj7</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1emtm6z</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t xml:space="preserve">it happened…😔 after 3 months of growth </t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1emtm6z</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1emtkvv</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>French with a touch of gold ✨</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0hl1m1cygchd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1emt85d</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Such a cute set my sister wanted 😍 it's so hard filing with no fingernail on your pointer I had to give up on making them even 😔 my huge bandage in the way lmao </t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1emt85d</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1emt4ot</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>The most satisfying press-on nails I've ever bought!! What do you think about them?</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1emt4ot</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1emrmkq</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I like pedicures, but I wish they’d leave my great toes alone. </t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1emrmkq/i_like_pedicures_but_i_wish_theyd_leave_my_great/</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1emq0xy</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>Need suggestions for similar colors</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1emq0xy</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1ems899</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>Asked for short nails charged for medium</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ems899/asked_for_short_nails_charged_for_medium/</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1ems6u5</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>new set!!!!!!!</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z6wn8e955chd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1ems3of</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cherry red coffin nails </t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lwq36w3f4chd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1emryvf</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>His and Her nails</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1emryvf</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1emrutk</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Inadvertently chose Poppi pink </t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vp0p68ob2chd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1emrqbj</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>Do you hate it too? lol</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1emrqbj</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1emre6x</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t xml:space="preserve">DIY: Can you spot the difference? </t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1emre6x</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1emraxi</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>from my studio :) I will be reading</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/izj956tcxbhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1emr9g4</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>Hi little guy🐝</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ufsuj4lhxbhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1emr962</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>Having a brat summer?!</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f3i0vpkfxbhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1emqsyn</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>Am I shaping my nails correctly?</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1emqsyn</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1emqf3j</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>First time question</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3hilofnoqbhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1emq1cf</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>Any Seattle people? Wife does nails at home</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gssbptnrnbhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1empzgt</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>Bridal Shower Nails by Me</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1empzgt</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1empvct</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My nail girl never fails me 💛 This is builder gel on top of my natural nails — Yellow with ‘glaze’ chrome 🍋 </t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1empvct</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1empau7</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>Finger paints "colorful collage" turned white?</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ixti3io8ibhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1emp75r</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How we feel about this vibe? </t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1yvaktaghbhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1emoswv</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>Milky Oolong 😍</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bl5gsqhjebhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1emor30</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I just got my nails done 2 days ago and I think they are lifting at the tips. I get them done every 2 weeks so can this wait until my next appointment? </t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a9n7u9j6ebhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1ely99r</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>Has anyone with a gel polish allergy been able to successfully wear acrylic nails?</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ely99r/has_anyone_with_a_gel_polish_allergy_been_able_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1emmj07</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What are these blue streaky marks on my nails (specifically thumbs)? </t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1emmj07</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1emnsfo</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>Fresh Biab Mani - chrome!</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yrlhoy067bhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1emnrkf</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>I'm in Love with this beach themed summer nail art</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1ifz79ew6bhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1emnp9h</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>My idea turned out amazing😙👌</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j2xyvp4j6bhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1emnaob</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The marble is on point </t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/klgy97zi3bhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1emmjos</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>New set… Good luck for the month of August 💅🏼😌🤞🏻</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kotv2505yahd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1emlu8a</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>Summer White</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3gxndea2tahd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1emlq2g</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>Fav longlasting press ons?</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1emlq2g/fav_longlasting_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1emliia</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>10 min nail art ideas...</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uuenolvrqahd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1eml9of</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>Press ons with the gel polish hack</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eml9of</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1eml94m</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A little black lacy mani for Vegas! </t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r32m2zxwoahd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1eml2xy</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fairycore press on set </t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dzyw21xnnahd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1emkxdo</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>Trying out gel tips</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xewbxpwkmahd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1emkj5a</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Rate this set </t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1emkj5a</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1emkqjo</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Jello Jello Peel-off base gel recalled? </t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5ztdk4r8lahd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1emkpde</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Love how holographic ILNP actually is! </t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1emkpde</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1emklco</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>My sister asked me to do her nails for back to school. Havent done nails in like 3 months! what do you think?</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1emklco</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1emkktj</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>Broken natural nail</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/thvg8yi3kahd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1emkeur</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Yes to droplets? </t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1emkeur</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1emkd09</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>Making my own designs ❤️</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0mbc2djliahd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1emk6cs</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>my first set of press on nails !</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1emk6cs</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1emk1gx</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>What do you think of this design? Do you like the color?</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cn0xgs4dgahd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1emiz2q</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>Stained toe nails</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/000ds3ry8ahd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1emit95</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>Question about clear coat</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1emit95/question_about_clear_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1emip4j</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Best gel brands?? </t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1emip4j/best_gel_brands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1emihr1</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t xml:space="preserve">do you see blue or purple? </t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1emihr1</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1emid6p</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>I may be newly single but ik my nail tech always got me 🤧❤️</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x2ydyon34ahd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1em9twc</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>A new salon in my country uses uv gel glue to stick translucent / opaque press ons to natural nails - is there any way this is safe?</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1em9twc/a_new_salon_in_my_country_uses_uv_gel_glue_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1emc0l1</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>Thin, foldable nails</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1emc0l1/thin_foldable_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1emegp5</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>Good resources for just nail polish nail art?</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1emegp5/good_resources_for_just_nail_polish_nail_art/</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1emiazg</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>Yall… my jojoba oil smells like bologna … AM I INSANE ????</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lybp557c4ahd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1emi93f</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Stained glass chrome nails </t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1emi93f</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1emhumz</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>First time getting a full set in years ❤️</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1emhumz</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1emckbc</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>Nails after removing acrylic . Normal?</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1emckbc/nails_after_removing_acrylic_normal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1emd8bg</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Did I buy a knockoff glass file? </t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1emd8bg/did_i_buy_a_knockoff_glass_file/</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1emdbzv</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>Gel nails turning yellow PLEASE HELP</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1emdbzv</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1emgzy1</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>My first time trying chrome nails - what do you think?</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1emgzy1</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1emgzxg</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>they’re so cute i’m in love &lt;3</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yskkb2i9v9hd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1emguha</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail growth and strengthening </t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1emguha/nail_growth_and_strengthening/</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1emgsiy</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>Had to share🐱💚✨💕🐾</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1emgsiy</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1emy9j1</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>Found my new Favorite Blue! 🤩</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n1c3yn5jpdhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1emy8qc</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>Looking for color Lumen and Etheral</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1emy8qc/looking_for_color_lumen_and_etheral/</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1emwwbt</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>{PR} Sassy Sauce | Polish Pick Up - Not your Mama’s fairy tale</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/d83epp7yadhd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1emvdth</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>Fluent in Fowl Language</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1emvdth</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1emv8vv</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>A skittle and a smoosh</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i3srerhcvchd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1emutm5</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Joker: Folie à Deux inspired nails </t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1emutm5</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1emueyh</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t xml:space="preserve">still wayyy too hot for cocoa, but i can have it on my nails! </t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2527ys01ochd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1emu2by</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>Shaping advice wanted, curved nails</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1emu2by</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1emu132</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>An Electric Eel in Love</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eq70pemrkchd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1emts3w</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help- Need Recommendations </t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1emts3w/help_need_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1emto4k</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>selling press ons</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o3grbqkqhchd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1emsnh7</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>First time doing french tips! They were so fun!</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1emsnh7</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1ems7wb</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My first time using jewels. So done judge 😋 I couldnt fit the last 2 legs of the spider. I think I did decent. </t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/naxsqric5chd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1emrg2m</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can you spot the difference? </t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1emrg2m</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1emrbto</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>Glazed Nail Fail</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z3ujo7k1ybhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1emra66</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>I'm addicted to velvet 😭</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/pnae203kxbhd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1emr4nj</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t xml:space="preserve">i heard we were doing bat summer </t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/znyne0hewbhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1emquvi</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>My Perfect Shell Pink</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l4wcuu96ubhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1empixo</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>Swatch wheels - can you reuse?</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1empixo/swatch_wheels_can_you_reuse/</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1empclq</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>Blue Velvet</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1empclq</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1emo4m4</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>When you can't decide on a colour, just wear both!</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1emo4m4</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1emnn42</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>Nailed it “Gloss Boss” and Kathleen &amp; co “Cherry Blossoms”</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1emnn42</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1emn3d4</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>Buying from nail supply</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1emn3d4/buying_from_nail_supply/</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1emkplu</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>My second INLP - Black Orchid</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1emkplu</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1emkg64</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>B(r)at Girl Summer</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/syml7l27jahd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1emkal1</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>First time trying ILNP, I'm in love</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p1m5e4l4iahd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1emjujo</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>Show me your cat themed nail art</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1emjujo/show_me_your_cat_themed_nail_art/</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1emiw5o</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>Mood ring and beginner nail shaping</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1emiw5o</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1emiioj</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>My holo</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/006tbk6s5ahd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1emi6f0</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>Layer experiment...</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/r5zulhqf3ahd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1emi68l</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>Alexa, play Adagio In D Minor 😔</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1emi68l</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1emhvqq</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cottage core combo </t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1emhvqq</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1emghjc</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>Mixing Shellac + stamping polish</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1emghjc/mixing_shellac_stamping_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1emfs2y</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>It’s giving cinnamon sugar glaze</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1emfs2y</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1emevp0</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>Just another Sour Apple Rings love affair</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1emevp0</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1emerf6</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>Any tips or tricks on creating a gradient?</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1emerf6</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1emedk4</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>This is the neon orangey red of my dreams</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7em81eibd9hd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1eme5t0</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>Rebottled my Mooncats</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eme5t0</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1emdrmw</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>That blue shift ☺️</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o63ccub599hd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1emcold</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>Kaleidoscope by El Corazon- Gemini</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1emcold</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1emchjm</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>Rogue Lacquer's Bread &amp; Butterflies</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/79znogesz8hd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1emblj4</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>Neon shimmers for late summer (Nuthatching a plan &amp; I'm a plover not a fighter, Bluebird Lacquer)</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1emblj4</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1embey2</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time buying Death Valley Nails and I love it! </t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/qemi1phir8hd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1emajxz</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>Monarch “Quantum Leap”</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1emajxz</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1eluyfg</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>First time going to a nail salon—this is after about 3 weeks!</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aexdqguub4hd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1em93x8</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gel nails </t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1em93x8/gel_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1em9cct</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>ILNP Flowerchild becoming silver?</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1em9cct</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1em6x43</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Chrome adjacent…. </t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1em6x43</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1emz2vk</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I did these today!! Acrylics </t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0zuozfdxydhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1emvyso</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Birthday set for a friend </t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/foaaqlz02dhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1emtmxf</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>selling press ons</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x7w7074ghchd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1emt8rw</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Such a cute set 😍 it's so hard filing with no fingernail on your pointer I had to give up on making them even 😔 my huge bandage in the way lmao </t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1emt8rw</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1ems61q</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New nail set and wanting opinions and pointers. </t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ems61q</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1ems3hx</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>my first attempt at 3D nail art! inspired by art from @dhton on instagram (ft. the mess in the background)</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ems3hx</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1emrevl</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t xml:space="preserve">DIY: Can you spot the difference? </t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1emrevl</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1emp26j</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t xml:space="preserve">marbled nails with metal paper by Evelyn Mejía </t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cu0sh14fgbhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1emovsd</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>Can you tell they’re press ons? 💚</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l18fcf24fbhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1emopma</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>Men’s Evil Eye Nail Design done by @ebonyroses_nailfactory</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1emopma</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1emnib7</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>Nails Kawaii 💖🐰</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hz7b07b35bhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1emn0jn</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t xml:space="preserve">best ideas try it </t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vaxffub61bhd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1emltng</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>Summer White</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7ga8nb3ysahd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1emlr6t</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>Favorite E-file??!</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1emlr6t/favorite_efile/</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1emioon</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>Butterfly nails 🦋</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yjpmis7z6ahd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1emi7ee</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>Stained glass chrome nails</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1emi7ee</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1emhvsl</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>Nowhere near perfect but for my first time, doing gel nails and doing nail art, I think they came out pretty good!</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1emhvsl</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1emeqlp</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>Where are my Breezy fans? Made these for the 11:11 Tour ✨</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1emeqlp</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1emep27</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>Busy month 💜</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1emep27</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1emdvmf</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Not posted for a while! My most recent sets i’ve created💜 </t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1emdvmf</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1emc9g9</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>I let the creativity flow freely with this one 💚</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4w6h0ci3y8hd1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Aug  9 08:09:53 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_08_11.xlsx
+++ b/data/2024_08_11.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C803"/>
+  <dimension ref="A1:C972"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14086,6 +14086,2879 @@
         </is>
       </c>
     </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1entxod</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>Pamper time ❤️</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1entxod</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1entw7s</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>had to indulge in a gold and pearl moment 🤍✨</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1entw7s</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1ent58j</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>How to fix?</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c9mm1b896lhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1enssgq</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>Nail Show Off! 🤍</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1enssgq</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1enqgq6</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>What are these paint pallets I’ve been seeing?</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1enqgq6/what_are_these_paint_pallets_ive_been_seeing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1enqesl</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>My at-home gel nails always fall off my thumbs</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1enqesl/my_athome_gel_nails_always_fall_off_my_thumbs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1enp7id</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>I FINALLY mastered rainbow cat eye gel ✨</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wo98v9bf1khd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1enseqp</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>I let the woman I’m going to “visit” choose the color of my nails!</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9yee9g3txkhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1enrtyw</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My favorite set this year so far </t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aa6hvisdrkhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1enqkrm</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nice design </t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/89d36cefekhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1enqjkk</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t xml:space="preserve">{PR} Sassy Sauce | Hella Handmade Creations | Never have I ever </t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9hwfuld2ekhd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1enqj87</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First attempt at extensions, shaping, and cateye </t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/i66206cydkhd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1enqe4o</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can you use gel polishes interchangeably? </t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1enqe4o</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1enq3cg</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pink </t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3qzt8qhs9khd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1enpwc9</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>First time manicure, I love how different it looks in different lights</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1enpwc9</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1enppu6</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>New set night glow ‘Lava’ I</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1enppu6</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1enpb6j</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Chrome Mermaid Nails </t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qxgk07vd2khd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1enpaov</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>I discovered nail wraps, and I never want to paint my nails again</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pclph0g92khd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1enp7ie</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>Star nails ⭐️</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vpo6bpof1khd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1enl38l</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>Why are my nails so oddly down-angled? Is there any hope for these hands? :(</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1enl38l</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1enkzlm</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>how do i get press ons off?!?</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1enkzlm/how_do_i_get_press_ons_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1enm830</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>nail help 😭</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1enm830</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1enone0</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t xml:space="preserve">what nail polish don’t melt off with sunscreen use? </t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1enone0/what_nail_polish_dont_melt_off_with_sunscreen_use/</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1enoerf</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>Iridescent Princess ✨</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/d5zjhgbdujhd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1eno9vq</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>favorite products to use for weak/brittle nails?</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eno9vq/favorite_products_to_use_for_weakbrittle_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1eno3c4</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>Which I love the most❤️</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eno3c4</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1eno0km</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Chrome on red &amp; gems 🌸 ✨ </t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/72zlutlwqjhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1ennn2i</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>Stilettozzz 😍</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/u4dxljvonjhd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1ennhaq</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Classic Red! </t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/01dwq7xamjhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1ennc4w</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>Festival ready</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bz54wul2ljhd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1ennc0v</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>DIY Cat Eye</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ojahc9xykjhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1enn0ot</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>Fav press on/glue on brands?</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1enn0ot/fav_press_onglue_on_brands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1enmvoa</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>Lil kitties 🥰</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1enmvoa</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1enmmtz</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>Nail techs: can you tell which hand is your clients dominant?</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1enmmtz/nail_techs_can_you_tell_which_hand_is_your/</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1enmjy9</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>Raindrop nails 💧</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7kqf05icejhd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1enm5yr</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Just got a pedicure and wondering how I can remove this stain? </t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8q4sss31bjhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1enm39u</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My creative spark is back </t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1enm39u</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1enlkg9</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>Finished painting a Deadpool nail for the Deadpool Wolverine nail set 🥰 I have some guns coming for him tomorrow haha and should I change the background? What colour 😖💕</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/k2yz2zqw5jhd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1enlf34</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>Natural long nails, what do you think?</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1enlf34</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1enlalc</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Summer Ocean nails 🌊 </t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iwllte2o3jhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1enl6xv</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>Simple and sweet summer nails with starfish accents</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s5umrbdl2jhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1enl0bs</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>So hard to draw the 🐜</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4urfxz2c1jhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1enkyen</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>What rating do you give to this effect?</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/673aselw0jhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1enkrej</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New set </t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wpfaeikazihd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1enkpxq</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>Abalone... sorta</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rqmbbs5zyihd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1enk67q</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>Nail Tech Appreciation Post</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qjnj64bmuihd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1eniyfd</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>Fake Nails for Nailbiting</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eniyfd/fake_nails_for_nailbiting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1enj95j</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cherry blossoms </t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1enj95j</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1enj55e</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>Butterfly nails🦋🦋</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1enj55e/butterfly_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1eniqfo</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>Husband did my nails for the first time 🥰</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/00zeqc3gjihd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1enikhj</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Summer Ombre 🌞 </t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jwjdfa68iihd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1enifl0</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Funky Vibes </t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1enifl0</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1eniboi</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Made new press on nails </t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eqnmrdhegihd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1enhkc6</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>stars and such stuff</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1enhkc6</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1enhe41</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>Does matte nail polish feel matte?</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1enhe41/does_matte_nail_polish_feel_matte/</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1enhc2a</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>Bubbles?</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xl7is0z09ihd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1engmvm</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>😁💅🏽</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4by541av3ihd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1enghcn</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>Press ons</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/60tizl3s2ihd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1engdgx</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I gave myself ring of fire and I’m so upset </t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4q5elj9z1ihd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1enfxe3</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>Atlanta Nail tech here….</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1enfxe3</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1enfwm5</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Summer vacation nails </t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oagmhe8jyhhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1enfn35</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Some of my fave sets over the last year. </t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1enfn35</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1enflbc</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>recent set, some cateye nails</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zhvv2z6bwhhd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1enezag</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>casino nails</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1enezag</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1enequ2</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>🌊Painted Polish Bait 'N' Switch ⛱️ The glitters are a perfect hint of sand and sea 😎</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1enequ2</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1enea1e</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>Went for something bright ☀️</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1enea1e</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1ene92m</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Should I take my acrylics off? Had them for about a week and a half. One is breaking. </t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ene92m</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1ene8dt</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>What shape would suit my hands?</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ene8dt</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1endvwn</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>kinda hate the colors</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/px05pi41khhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1end280</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>Today I got French nails</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ulzdpog5ehhd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1encpwr</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>Nude colored stilettos</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1encpwr</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1encoa1</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>Do we like these??</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1encoa1</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1encmc6</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>First attempt at wearing press ons</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1encmc6</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1en9xow</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>My light blue nails, natural length, kapping gel 💙 artist IG @rogallardonails</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jrx22uzzrghd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1en6ybu</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>my nail as a waitress</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vxr9v6nq6ghd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1emzzol</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Why is my Neonail manicure always lifting ? </t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/otrsgw2m9ehd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1en72ju</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t xml:space="preserve">loving the fruit nails trend so much </t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v22omkik7ghd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1en8avo</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>UV/glow swirlies</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1en8avo</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1en8yty</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>Avoiding skin when painting nails</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1en8yty/avoiding_skin_when_painting_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1enad1z</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>New set, part me is debating on the water color one even though it's exactly what I asked for lol</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1enad1z</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1enans6</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>How should I design my nails?</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1enans6</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1enaqou</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>did my own dip nails</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/urrd9ctoxghd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1enb8q4</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>Summer nails🍊🍋🍋‍🟩</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1enb8q4</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1enbyo7</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>First marble in years.</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hklsujte6hhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1enbs2e</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>🍓 birthday nails!</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1enbs2e</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1enbruh</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>natural</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2n771u625hhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1enbpdx</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>What is Gel X and why is everyone doing it lately?</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1enbpdx/what_is_gel_x_and_why_is_everyone_doing_it_lately/</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1enbf90</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Loving this color </t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b983jwzi2hhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1enat2j</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>Square has my 💓 lately! Natural nails with gel overlay and gel polish :)</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l3ke2kg6yghd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1enaspj</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>In honor of my name I got fruit nails! I am jucyfruits🍒🥝🍇🍋🍉🫐🍌</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qivwty44yghd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1ena9hp</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>Bug nails I did! Too weird?</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/csmn3e7dughd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1en9yp3</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Natural Nails - My last Summer set! </t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6oycvm57sghd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1en9oxu</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>Bees 🐝♥️</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1en9oxu</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1en97ey</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>💚🕸️</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cf0644etmghd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1en94p1</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>Summer fun sharky set!</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1en94p1</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1en8x04</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>Basic b*tch "Rosa" as they say in Germany :)</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1en8x04</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1en7yix</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>Going to nail school as a mother of two?</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1en7yix/going_to_nail_school_as_a_mother_of_two/</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1en7sbb</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>New selfmade 🫶🏻my bf picked two random colors. Luckily they matched together 🥳</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j8wghi4rcghd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1en7bpc</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>Orly “In the Conservatory”</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1en7bpc</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1en7a57</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>My favorite set yet ✨</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1en7a57</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1enskv6</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>My neighbor put out Halloween decor…</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1enskv6</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1ensa5m</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>shaping tips?</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ensa5m/shaping_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1enr8bg</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t xml:space="preserve">polish bottle top closing unevenly </t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kcf95g84lkhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1enr7nf</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>nail adhesive tabs!</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1enr7nf/nail_adhesive_tabs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1enqkmg</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t xml:space="preserve">{PR} Sassy Sauce | Hella Handmade Creations | Never have I ever </t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1enqkmg</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1enq41n</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>Moody Summer</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1enq41n</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1eno0g2</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>DVN “Two Ticks and No Dog”</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eno0g2</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1ennrdo</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>Last week of summer weather</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nmk6y63eojhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1enni8q</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>When your LynB and Beyond Polish orders come on the same day 😮‍💨</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4h9teekjmjhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1enmgcj</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>Tenta-Cool 💜💙🐙</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1enmgcj</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1enlqmc</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>Some recent cheapie manis</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1enlqmc</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1enl2jo</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>Most interesting finish I have in my collection (Sense and sensibility, Rogue lacquer)</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bgfvo1st1jhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1enkv5m</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>Saffron Jelly</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1enkv5m</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1enkuht</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>finally jumped on the horseshoe magnet - worth it! ✨</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/oafcijizzihd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1enkqyf</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Goblins and ghoulies squad assemble </t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1enkqyf</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1enkjoo</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>Anyone try this? How is it?</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/datlkvolxihd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1enk9jh</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Polygel recommendations? </t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1enk9jh/polygel_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1enjx60</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>I need a dupe for TheDonDeeva's The Choice iS Yours!!!</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1enjx60</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1enji58</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Girl Scout nails </t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1enji58</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1eniqjx</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>Haunting Your Own House - Emily de Molly</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eniqjx</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1enigx3</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>Deep space ☄️</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1enigx3</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1enif4v</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>My first DIY crelly</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5fmdww24hihd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1enhsqz</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>Get Lobstered is crazy</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1enhsqz</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1enhs9v</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>Oh the heartbreak of a bad nail break. Been growing them for months and now my pointer looks like it got a bad buzz cut. Lacquer is Petals from a Narcissist by Mooncat</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zhm1odidcihd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1enfn2d</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>Didn't mean to go so heavy on the flakes 😅</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x3dgu0mowhhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1enfg4y</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>About to take the plunge... (And try a new nail shape)</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1enfg4y/about_to_take_the_plunge_and_try_a_new_nail_shape/</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1enews8</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Metallic Mega Mix Collection </t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1enevj4</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1enespz</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>I LOVE LAYERING COOL POLISHES!!!1!!!!!1!1!1;</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1enespz</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1eneq8c</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>🌊Painted Polish Bait 'N' Switch ⛱️ The glitters are a perfect hint of sand and sea 😎</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eneq8c</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1ene4v9</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>Birthstone nail polishes?</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ene4v9/birthstone_nail_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1endsmf</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>Truth or Dare with a lil’ Butterfly Effect</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1endsmf</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1endryo</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>🍓 gel mani!</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1endryo</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1endc1v</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How I love a good blue glitter </t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/66qorcs4ghhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1encgbh</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Added to my order at the last second because my BF loved it... just put it on and now I feel like the coolest alien on the block! </t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/p83ernou9hhd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1encbxl</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>Gel x - Is it safe?</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1encbxl/gel_x_is_it_safe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1enc5mu</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>How does nail oil work with nail polish on?</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1enc5mu/how_does_nail_oil_work_with_nail_polish_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1enb6wd</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>Why lacquer vs gel/dip etc</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1enb6wd/why_lacquer_vs_geldip_etc/</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1enap56</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>la vie en bleu 🧿</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1enap56</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1ena3dx</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>Mooncat Treachery in the Blue 😻</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/62exeyv4tghd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1ena1ip</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>ether dragon (at the hair salon)</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ena1ip</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1en9o4b</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Freshly Bitten - Mooncat </t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1en9o4b</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1en93ki</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t xml:space="preserve">first magnetic polish and i’m in love tbh </t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/h38zzdq1mghd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1en84iq</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>Short, red and messy ❤️💅Anyone else dilutes their goopy polishes with polish remover and rubbing alcohol? I know it's bad but so far it's working 😬</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1en84iq</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1en6iku</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>People in the EU: Where do you buy this?</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0feurmy93ghd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1en5h1u</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>Purple Polish (These aren't my nails)</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2fhddpjevfhd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1en51lc</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What is your favorite gel polish brands in EU? </t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1en51lc/what_is_your_favorite_gel_polish_brands_in_eu/</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1en50l8</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I’m sorry— it’s another Goblins and Ghoulies post </t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/y6kri2sprfhd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1en4wo1</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>Flakie topper madness</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1en4wo1</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1en17zx</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>I miss the winter.</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7puf4gctoehd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1entvym</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>Syrup nails, thoughts?</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7kjzzf6cflhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1enra5b</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>What can I do to improve?</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1enra5b</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1enr8zk</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>New set! No gel/acrylic just clear extensions, regular polish and glue</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1enr8zk</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1enqmz8</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>True artists in this sub</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1enqmz8/true_artists_in_this_sub/</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1enqhka</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>First attempt at extensions, shaping and cateye</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/b41y54nhdkhd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1enpb0c</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>Expectations vs Reality</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1enpb0c</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1enp1bq</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>Another set completed so fun!</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1enp1bq</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1enlpn4</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>a picnic vibe for summer</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/dhwutui37jhd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1enlk6t</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>Finished painting a Deadpool nail for the Deadpool Wolverine nail set 🥰 I have some guns coming for him tomorrow haha and should I change the background? What colour 😔💞</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/egdsjixt5jhd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1engn0f</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>Summer nails</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a2zg3i6w3ihd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1enfgoj</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>Anyone printed nail wraps?</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1enfgoj/anyone_printed_nail_wraps/</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1enezsr</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>casino nails</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1enezsr</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1eneddo</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Art </t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/55jqzzb3nhhd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1endvzd</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Do you also love sparkles and stars? </t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/itemoiq1khhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1enbx0h</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>Silver nails🪩🩶</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/023agex26hhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1enbrlw</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>product advice for a beginner?</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1enbrlw/product_advice_for_a_beginner/</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1ena7te</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>I love how this set turned out 🪩🦋🩶</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ena7te</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1en45op</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>Nails I did this week!!</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1en45op</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1en3mal</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>Should I let my newly painted press ons sit?</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1en3mal/should_i_let_my_newly_painted_press_ons_sit/</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1en3jq5</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>What do you use as a nail stand?</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1en3jq5</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Aug 10 08:08:27 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_08_11.xlsx
+++ b/data/2024_08_11.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C972"/>
+  <dimension ref="A1:C1126"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16959,6 +16959,2624 @@
         </is>
       </c>
     </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1eon6bs</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>💟 being a nail tech is fr such a dream I love itttt</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8sddg1p6gshd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1eomy8o</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>💐🌺🌸</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eomy8o</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1eomsyy</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Watermelon nails 🍉 </t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6c53t87wbshd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1eomrca</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>Pink croc blooming gel</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eomrca</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1eomeey</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>Nail day</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eomeey</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1eol55b</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t xml:space="preserve">She wanted a "french heart" </t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j65cgvt7trhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1eokn9c</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>Accidental Awesome!</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lumtugh3orhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1eok68k</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>💜</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ld7nyaibjrhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1eojv5q</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>COQUETTE NAILS🎀🩷</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6t6n3cfagrhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1eojswq</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>Letting Nails Breathe?</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eojswq/letting_nails_breathe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1eojre4</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>Gel Art Neccessities?</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eojre4/gel_art_neccessities/</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1eojq2f</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>That pink gradient is just right for summer!!🩷</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9l8j8475erhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1eojje9</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>Hard Gel Overlay ✨</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eojje9</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1eoj873</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>ehh</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jfha6o6x9rhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1eoj7ar</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>first time doing marbling...thoughts?</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eoj7ar</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1eoj0n4</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>black heart 🖤🖤🖤</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eoj0n4</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1eoiy4a</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>Still Amazing 💜</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eoiy4a</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1eoimmq</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Bye bye blue… </t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h30tih1g4rhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1eoiaya</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>New set, in love</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7how3lgh1rhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1eoi1rf</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>went simple &amp; shorter this week 🩷✨</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c1cuzln6zqhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1eohlwz</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>One of my favorite sets maybe ever! 🩵 Marbled turquoise with a few frenchies and dreamcatchers! My nail tech is an artist! 🎨</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eohlwz</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1eohcvr</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>Nail growth time lapse</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/08tcph2tsqhd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1eoh0yg</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My nail service was in my favorite color, would you do them? </t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dx44j9btpqhd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1eoghy8</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Why don’t more nail brands do brand apparel?  </t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eoghy8/why_dont_more_nail_brands_do_brand_apparel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1eoga09</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Eggs Nails </t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vjiitbq3jqhd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1eog8vi</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t xml:space="preserve">cherry nails for the summer!🍒 </t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fy6j9qmviqhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1eog2eb</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>Learning how to build an apex</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hye4f92bhqhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1eofsl5</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>Draculaura nails I did the other day 🩷🖤</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jyhq08ayeqhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1eofqtc</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>Help with cuticles?</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/57g2ojpieqhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1eofjje</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>Summer color ✨</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dfi1dduqcqhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1eofc73</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>PLSS I NEED HELP</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eofc73</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1eof9q7</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>it’s never too early for halloween 🎃👻</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eof9q7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1eof8ts</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>Looking for press on suggestions - long length, solid colors?</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://www.kissusa.com/products/kiss-gel-fantasy-sculpted-nails-cosmic?nbt=nb%3Aadwords%3Ag%3A20338490116%3A150455824029%3A664469943334&amp;nb_adtype=pla_with_promotion&amp;nb_kwd=&amp;nb_ti=aud-876394266452:pla-2224365889387&amp;nb_mi=113847068&amp;nb_pc=online&amp;nb_pi=FS28X&amp;nb_ppi=2224365889387&amp;nb_placement=&amp;nb_li_ms=&amp;nb_lp_ms=&amp;nb_fii=&amp;nb_ap=&amp;nb_mt=&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=KISS%20Nails%20%7C%20Sales%20%7C%20Shopping%20%7C%20Nails%20%7C%20K23OCMDM001&amp;utm_content=664469943334&amp;utm_term=&amp;gc_id=20338490116&amp;h_ad_id=664469943334&amp;campaign_id=20338490116&amp;gad_source=1&amp;gbraid=0AAAAADhsL2acqMZx1V7o86nc9jGmqqu0I&amp;gclid=CjwKCAjw_Na1BhAlEiwAM-dm7CcfjkC3jOIc5T97PJNbXW7fi26S2xZvOqsHMKzyycxJIIpy4RSMLBoCT5oQAvD_BwE</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1eof2h3</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>Adesse Age Defying Nail Treatment</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/95abot5p8qhd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1eoehi1</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Do these look like obvious press ons? </t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eoehi1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1eoe9t8</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>sanrio halloween press ons🎃💜</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j262xke92qhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1eodx2w</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>my newest set!!!</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c4le6ijizphd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1eodx25</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>Please convince me these aren’t bad</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vvnqr4yhzphd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1eoduhg</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>Do these press ons look ok?</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ahwqlufyyphd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1eodpxm</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>I wanted a bright color 😂😂😂😂</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eodpxm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1eodh7a</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>The worst manicure I’ve ever had.</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eodh7a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1eodg2f</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cut my press-on to start removal but they look kinda cute short?? </t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eodg2f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1eoce8e</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>Is this shape ok?</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wyua5zk4ophd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1eobh9m</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Loved this color but someone said it reminded them of pea soup and now I can’t unsee it😭 </t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eobh9m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1eoba48</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>Crooked Acrylics</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eoba48</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1eo887o</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>Nail DIY or Salon?</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eo887o/nail_diy_or_salon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1eo9ybu</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My first self made gel x nail </t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ujkcgyxc6phd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1eo9ngw</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>A new way to paint my nails?</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eo9ngw/a_new_way_to_paint_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1eo902v</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Just did my non dominant hand! (i painted the house earlier today hence the white paint on the hands) </t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g8ps73eazohd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1eo8xyi</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>{PR} Sassy Sauce | Juicy</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eo8xyi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1eo8oyf</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Yellow! </t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ga1v0kjzwohd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1eo8c5w</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>I keep finding packaging that matches my nails ☺️</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eo8c5w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1eo7pm6</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>It’s giving ✨hypoxia✨</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c4ahfmwspohd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1eo7c2g</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t xml:space="preserve">love my nail guy! </t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eo7c2g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1eo6boi</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>Practicing! First time doing this</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eo6boi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1eo5az1</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t xml:space="preserve">French manicure after almost a year and a half </t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c7q7jtsd8ohd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1eo5972</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>I'm back from Mexico and matching manis with my daughter!</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eo5972</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1enu64h</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>What are your thoughts on these?</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1enu64h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1entkbs</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>Which press on is the right size?</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1entkbs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1eo3zbh</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>Static Nails Question</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eo3zbh/static_nails_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1eo4lzs</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>Fresh mani</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ow6cbpme3ohd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1eo4boh</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>[Male] Advice for thick Hands</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eo4boh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1eo45qa</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t xml:space="preserve">So cute!🥰 </t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eo45qa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1eo3z0h</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>Russian Mani Question</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eo3z0h/russian_mani_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1eo2r4s</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>First time i got my nails done - porcelain</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fvag3llmqnhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1eo2kih</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>I made some custom press-ons for some friends who are getting married! What do you think?</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eo2kih</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1eo23d2</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>Critique/Tips</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eo23d2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1eo0y82</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>Contemporary delicate design 🎀</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/iuuvjtrqdnhd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1eo0ihv</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>I ❤️ Pink So Much</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3c1y7ykganhd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1eo0e3i</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>New to stamping - latest try</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eo0e3i/new_to_stamping_latest_try/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1eo0cyp</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>Friday Blues</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4mo7ijgd9nhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1enzroh</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>This weeks set🥰</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1enzroh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1enzf82</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Best quality (non-gel) clear topcoat. </t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1enzf82/best_quality_nongel_clear_topcoat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1enyc0c</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I truly cannot stay away from glitter. </t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/svbaku1ysmhd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1eny454</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>Do you like these?</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eny454</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1enxzgr</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>Looking for advice about gel nails</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vqpsglstpmhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1enxm4l</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>Neutral gel nails, I love colours and nail art but I get so bored fast when I have it</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1enxm4l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1enwjo1</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>Press on Nails ✨️</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2wax2tf8bmhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1enwdjk</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>First time doing nails! (a set for my mum 💞)</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1enwdjk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1enwbmy</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>✨✨ my new set</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zze97sdp8mhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1enw9f7</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>Can’t beat classic black 😍🔥</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/c9k3tos08mhd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1enw8cl</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>Not a cursed pose, but a cursed style!</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pjzcncqn7mhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1envwes</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>Want to create nail content, what do you think of my nails ?</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/w15xie5w3mhd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1envho2</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>Need your nail recommendations for an all-black suit</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1envho2/need_your_nail_recommendations_for_an_allblack/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1envfy8</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>I'm not a huge pro or anything, just a girl who likes to do her nails &lt;3 I'd appreciate tips on how to improve!</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xvxk9jegylhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1envfrm</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>second set ive done on my nails! 🎀</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1envfrm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1enueeq</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>My take on kawaii junk nails 💖 (less junky so they're more practical)</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1enueeq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1eola7z</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Recovering nail biter </t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eola7z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1eoj4m2</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>painting nails, but not?</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1eoj4m2/painting_nails_but_not/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1eohzuf</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>What happened to Jelly Apple from essie?</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1eohzuf/what_happened_to_jelly_apple_from_essie/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1eogval</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Watermelon - the longest I've grown out in a while </t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eogval</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1eofy9x</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>Help! I can’t find Cirque Rosewater Jelly anywhere! 😭</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1eofy9x/help_i_cant_find_cirque_rosewater_jelly_anywhere/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1eofw67</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>Ready for a beach weekend 🐚😎</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7d7pvmzrfqhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1eofni2</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>Tallulah helping me show you my nails. Undiluted this time I promise 🥲</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eofni2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1eof3rk</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>Anyone else like stained nails?</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1eof3rk/anyone_else_like_stained_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1eoemrl</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>Spyglass</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eoemrl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1eoelg8</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>My first attempt at a french tip (so i could match my cat)</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xabq37ls4qhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1eoec26</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>Nail growth time lapse</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/znteznvq2qhd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1eoea9z</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>Contact Dermatitis from Beetles Nail Glue, Alternatives?</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1eoea9z/contact_dermatitis_from_beetles_nail_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1eoe8r2</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>Orly Are You Sherbert?</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eoe8r2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1eoe02j</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>Spirit me away!🐉</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eoe02j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1eocqoe</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>Rocketman</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eocqoe</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1eocpy3</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>Velvet skittle 🌈🦄🍭</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eocpy3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1eocpru</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>Skittle time!!!</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eocpru</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1eobxrm</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>I broke a nail and had to cut them off to match!</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e96u8giqkphd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1eobh0v</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>First time doing a glitter gradient 🤩</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rmjnvsnchphd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1eobghy</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>Got a gel manicure removed yesterday and there’s a weird spot on my middle finger…does anyone have suggestions for products to take care of the spot?</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nr3h1ci9hphd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1eob8tg</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>How to do it better?</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eob8tg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1eob6yb</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>blu mood</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3pcfuzhbfphd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1eob2iw</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Any Baldur's Gate 3 Fans in the Audience? </t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://youtu.be/sMX_VnaIMI0?si=yEu80macSF9sUxBa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1eoag33</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First Attempt at frenchies </t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iej3k4ex9phd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1eoabo8</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>Mooncat River Styx vs Polished for Days Shockwave</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1eoabo8/mooncat_river_styx_vs_polished_for_days_shockwave/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1eo9wa9</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Same same but different </t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pas7iw7y5phd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1eo9q4o</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>Party Animal + XOXO Jelly</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eo9q4o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1eo976p</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love a yellow polish 💛💗❤️💛 </t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eo976p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1eo964x</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>Did I find another Marshall’s/TJMaxx-only Orly?</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eo964x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1eo90q2</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>{PR} Sassy Sauce | Juicy</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eo90q2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1eo8e6o</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>nails match my tacos 😈🌮</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gvvc0k7tuohd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1eo828h</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>It's giving toothpaste ✨️</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eo828h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1eo7wft</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>DVN x Mooncat combo 🏜🐈</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/s639nua9rohd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1eo7ex2</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>Sour Apple Rings</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eo7ex2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1eo7dsr</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Finally successful at warer marbling!! And some flowers 💐 </t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eo7dsr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1eo7buz</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>Y’all!!!! I’m matching😂</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eo7buz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1eo6flj</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>HELP! Flower Child vs Blue Bell vs Fairy Dust</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1eo6flj/help_flower_child_vs_blue_bell_vs_fairy_dust/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1eo6bok</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>The camera does not do this color justice 😍</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eo6bok</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1eo66a2</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Here’s a dupe for Ethereal - Ethereal Vampire! </t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/32m4atfpeohd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1eo652e</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>What would you add to this? Crème pink/red neons!</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6r9uluggeohd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1eo611h</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>neon has me falling in love with crèmes</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eo611h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1eo59ts</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>Now THIS is how you do a lime green!!</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lapvbu958ohd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1eo4jox</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>My first not-completely-failed decal. I wish my thumb had more real estate, because on the mat 𝖎 𝖙 was clearly consuming planets</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t7m7pk4y2ohd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1eo45o9</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Death Valley Nails! </t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eo45o9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1eo3r8o</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>Okay to go to salon?</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eo3r8o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1eo2nze</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>Purple shifty beetle wing skittle</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/i1m7tk31qnhd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1eo2ilf</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>Can someone explain to me how many coats of what products to use?</t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1eo2ilf/can_someone_explain_to_me_how_many_coats_of_what/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1enzybn</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t xml:space="preserve">UPDATE TIME!!!! </t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1enzopw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1eny1ai</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>advice for lasting press ons</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1eny1ai/advice_for_lasting_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1eom5xs</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>what do u think</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dca8y3sh4shd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1eoktxm</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Press ons I made 🍒 </t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eoktxm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1eoi1hw</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ISpy inspired set I did for myself </t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eoi1hw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1eohm3d</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Did my moms nails for back 2 school! </t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eohm3d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1eofrgh</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>Draculaura nails I did the other day 🖤🩷</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rl74buzneqhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1eoer6v</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>I have been obsessed with painting these pretty little hibiscus flowers lately 🌺</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eoer6v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1eoe984</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>Side wall pooling</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eoe984</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1eocdb3</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sparkling Strawberry Nails </t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n1xxy3gxnphd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1eocd93</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cartoon nails </t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v32pjzaxnphd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1eoa1d0</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>🌊🏖️ I'd wear this set for a beach vacation</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eoa1d0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1eo9caj</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>second time ever hand painting lettering.. opinions?</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eo9caj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1eo7ueq</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>I like them, but I didn't love the shape, do you think I should change manicurists? or give it another chance? (I'm embarrassed to tell him that I want the most stylized shape because I had already told him so and I just smooth them out a little more) help</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eo7ueq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1eo5uks</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>Perfect nude?</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eo5uks</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1eo4zvv</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>My try at aqua nails!</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/y123b9676ohd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1eo4f25</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>what do u think</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u4uipmh12ohd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1eo2nvq</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>Babyboomer with 3D flower🌸🩷</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1exzv9c0qnhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1eo22ae</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Critique/ Tips </t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eo22ae</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1envin8</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>Need your nail recommends for an all-black suit!</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1envin8/need_your_nail_recommends_for_an_allblack_suit/</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Aug 11 08:08:09 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_08_11.xlsx
+++ b/data/2024_08_11.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1126"/>
+  <dimension ref="A1:C1299"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19577,6 +19577,2947 @@
         </is>
       </c>
     </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1epeb6k</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>Can yall help me find this gel polish?</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1epeb6k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1eped86</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t xml:space="preserve">did my sisters nails for her 14th birthday </t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eped86</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1epdzpv</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>Suggestions</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1epdzpv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1epdpq0</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t xml:space="preserve">i luv a simple french </t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s5oiom8t6zhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1epd2m8</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>Got my nails done today🩵</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v5zuaxrozyhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1epbtlo</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Vegas Nails 🎰🍾 </t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1epbtlo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1epbrss</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>Lil jellies</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tecuovn1myhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1epbnfq</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>new manicure</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1epbnfq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1epbi29</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>What are some major red flags for a nail salon or artist in the process of doing nails?</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1epbi29/what_are_some_major_red_flags_for_a_nail_salon_or/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1epbev4</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>Young Nails gel polish</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1epbev4/young_nails_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1ep94hr</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>Custom $uicideboy$ and TØP’s inspired sets i got commissioned to do!!!</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ep94hr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>1epb1k3</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>New set</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1epb1k3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>1epazg8</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Zombie Claw - My Poopsies </t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1epazg8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>1epa836</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>Pretty in Pink</t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xgmeve617yhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>1ep9vts</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>Painted my nails to look dirty</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ep9vts</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>1ep9udi</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t xml:space="preserve">before 👉🏻 after 🌹 </t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ep9udi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>1ep9qiu</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>🍒✨</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ep9qiu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>1ep9oq1</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My best guy friend let me paint his nails </t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ek2i0fxu1yhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>1ep6dc3</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>Press on nails??</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ep6dc3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>1ep8950</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t>Vamp Nails</t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ep8950</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>1ep7hji</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t>Gel</t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/udz14tbehxhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>1ep6ybd</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My fav ones up to date </t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ep6ybd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>1ep6xrz</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Last days of summer set! </t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ttkwm5ejcxhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>1ep63oe</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t>Regular polish help pleeeease</t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ep63oe</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>1ep63h1</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>My bf always takes me to get my nails done when we go out of town for drill 💕</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ep63h1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>1ep5kkw</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>Peridot inspired nails in true Leo fashion</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/e18nnj031xhd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>1ep5y09</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>Question About French Tip Fills</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ep5y09/question_about_french_tip_fills/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>1ep4dt1</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Got these nails for my sisters 21st birthday! </t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3vuqu1n4rwhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>1ep5rzy</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>How much would you pay for this gel set?</t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ep5rzy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>1ep5nro</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>New colour for today!</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iiwvgvqs1xhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>1ep5f73</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Did these today! </t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hodftlwtzwhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>1ep5bgw</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>BEEzz... used rubber base and stamping plate/polish, matte top coat. 🐝🍯💛 They look nicer in person than pics.</t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ep5bgw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>1ep568u</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New set 💅🏻 Back to red </t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ep568u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>1ep52wk</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>Howdy</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i6c5w5hxwwhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>1ep4xpa</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>New Color 💜</t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5bx65gwjvwhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>1ep4mcl</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My Sweet Piano set I did! </t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ne9yj583twhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1ep4bbv</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t>Love this set 🍋🤍✨🕊️🌼</t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xpg1b1ujqwhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>1ep46i8</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Press-on nails </t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ep46i8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>1ep3zd4</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Love my nails... wished they photographed better 😪 </t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ep3zd4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>1ep3y1h</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>Is this normal/usual with gels?</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dtpdp1eknwhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>1ep3pwp</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>how to have longer nail beds</t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ep3pwp/how_to_have_longer_nail_beds/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>1ep3e58</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>Fresh set for my client do you like these?</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kc6xno22jwhd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>1ep1xja</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t>What I got VS What I Asked For, inspo pic from @leylasbeautystudio on IG</t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ep1xja</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>1ep36kl</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t>Should I give up on them?</t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ep36kl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>1ep2z7u</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t>🩷</t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8tr6mqalfwhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>1ep2yfz</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>Natural Nails</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ep2yfz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>1ep2qon</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>Spider nails🕷️🕸️❤️🩵</t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vvn0it6odwhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>1ep2knr</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t>Thoughts on my edgy man-french?</t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ep2knr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>1ep26dk</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How cute are these encapsulated flowers? </t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ep26dk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>1ep1xqz</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>My second time hand painted lettering!</t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/19223mk57whd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>1ep1n3t</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>At home gel</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ehrcdy4r4whd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>1ep1c0g</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>Can I get a fill with dip???</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ep1c0g/can_i_get_a_fill_with_dip/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>1ep1noy</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time doing gel X how did I do? </t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ep1noy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>1ep1bvo</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I am trying to stop biting my nails, so used some clear press ons, painted them and added some decals... My friend told me it's too feminine but idgaf, like skulls are suddenly feminine? Nah, my daughter thinks they are nice and that's all the criticism I need!! </t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ep1bvo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>1ep0zru</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Design done in 3 hours, what do you think? </t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lvnfl4jgzvhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>1ep0pxm</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>First time doing a gel mani on my short nails</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ep0pxm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>1ep0ijm</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t>I feel like my base coat is too clear…</t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ep0ijm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>1ep0k3j</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t>Got my nail station set up!</t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/txdyncq0wvhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>1ep0gn2</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>All mine ALL REAL wish I had a nail tech in my area</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ep0gn2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>1eozw46</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>RIP middle finger nail! 😭</t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xws6923qqvhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>1ep08e5</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>my favorite color for my feet 🫶🏼</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rszz0eketvhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>1eolf1q</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t>I posted the pic of the yellow chrome nails, for reference on my typical style; here’s my last set!</t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eolf1q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>1eor03z</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>Help- dropped a literal hammer on my toe</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eor03z/help_dropped_a_literal_hammer_on_my_toe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>1eouses</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>how do you get opi gel polish without being a salon?</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rewr6xrhnuhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>1eovs7u</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>Lovin my latest set 🥰 inspired by another set I saw here ❤️</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eovs7u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>1eoz809</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>Bliss Kiss Cuticle Oil- what the heck is with the price???</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eoz809/bliss_kiss_cuticle_oil_what_the_heck_is_with_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>1eoyyqi</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My first time getting gel nail art done and I love how they turned out! </t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eoyyqi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>1eoywze</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>Art nails</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yg97ep45jvhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>1eoyw1g</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>Simple and cute 🩵</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rtncv3hyivhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>1eoyt4h</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t>Blue glitter jellies</t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u9r86s0civhd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>1eoyozg</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Adventure Time </t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x6ee83rbhvhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>1eoym8j</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t>Birthday Nails</t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z6dl1u1ugvhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>1eox3ll</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>Look at the growth of my nails</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eox3ll</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>1eoxshy</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>Playing around with stickers. Shrimp nails.</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4gp7h2yjavhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>1eoxnwc</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t>Modern day french tip with glitter ✨</t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uy2w5fzk9vhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>1eox3j3</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t>My prom nails 🖤✨️</t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eox3j3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>1eowzka</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Do the glittered edges seem jagged? </t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eowzka</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>1eowryt</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t>Back to school that i freestyled designed 🎀</t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eowryt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>1eowpw4</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Press ons </t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eowpw4/press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>1eowkx4</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First attempt at aurora nails </t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rtfwdouq0vhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>1eowgqx</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t>From myself to myself 🥰</t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0eygez9g0vhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>1eow2ro</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>Did some experimenting at home!</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eow2ro</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>1eovrbc</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t>New set of gel nails. Thoughts?</t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eovrbc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>1eouqs3</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t>Halp</t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eouqs3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>1eoucb7</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t>My first acrylics... I wanted to blend it over 5 colors, but the shop had been closed for 30 minutes already and they were pushy... so we did 3.</t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eoucb7/my_first_acrylics_i_wanted_to_blend_it_over_5/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>1eotw22</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t>Classics. But I love them</t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qm32a1a9guhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>1eosovj</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Wedding nails! </t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/40vsenu36uhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>1eosgk8</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t>How long are my nails? Some people think it's dangerous 😅</t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eosgk8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>1eosd84</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t>Total beginner needs help</t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eosd84</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>1eos9p4</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t>One of my favorite sets so far</t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eos9p4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>1eos4lu</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Back to press-ons! </t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xpyjgwa41uhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>1eorr0g</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t>1€ - had to shape them though</t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eorr0g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>1eord5u</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t>Are they pretty? 🤔</t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ggr03ndvtthd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>1eopznr</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Using acrylic as a barrier </t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eopznr/using_acrylic_as_a_barrier/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>1eopi12</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t>Got these done a while back on my bday 🎀</t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xtaddwt19thd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>1eoodrn</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t>💟💟💟 purple nails.</t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eoodrn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>1eoo6n9</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t>I feel like something is off</t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eoo6n9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>1eonug1</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t>My Red Nails!</t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aylzifbaoshd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>1epcmfo</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t>Absolute best magnetic/cateye gel polishes?</t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>/r/lacqueristas/comments/1ep8ume/absolute_best_magneticcateye_gel_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>1epbl1m</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t>Impossible to photograph ‘nearly blacks’</t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1epbl1m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>1epb4i5</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Zombie Claw - My Poopsies </t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1epb4i5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>1epaqtc</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>Best Deep Ridge Filling Base Coat?</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1epaqtc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>1ep9uww</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t>Quick dry top coat - with a long brush?</t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ep9uww/quick_dry_top_coat_with_a_long_brush/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>1ep9uak</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>What does “marketing teak nails mean”?</t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ep9uak/what_does_marketing_teak_nails_mean/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>1ep9ptg</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>Stunning BKL freebie</t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ep9ptg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>1ep8kpv</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hear me out: ILNP Lily over Flower Child </t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/gwpfk51crxhd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>1ep8fez</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t>The durability of press ons</t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ep8fez/the_durability_of_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>1ep83vp</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t>Sugarcoat Everything - Sassy Cats Lacquer</t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/umz011wymxhd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>1ep82lu</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t>Would love some help :)</t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3f3ygxvqmxhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>1ep7rl5</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t>Dupe help needed! OPI All is Berry and Bright</t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ntmph8ayjxhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>1ep7m1s</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t>This sub made me do it…</t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ep7m1s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>1ep7hot</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Adventure Time </t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ep7hot</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>1ep7ea8</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I’m very picky with pinks, but this color is stunning. A Heart’s Heavy Burden </t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ep7ea8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>1ep74q0</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t>I’ve been sleeping on this shade for so long</t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3x13gpy6exhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>1ep5ysh</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t>Im growing my nails and I have those annoying lines on my nail plate(?) (Not sure what it's called). Are they normal?</t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ep5ysh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>1ep5728</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t>Swooning over my first ILNP polishes!</t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d8jndo2xxwhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>1ep4tsf</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t>This is what mooncat bottles are supposed to look like (mc smokescreen)</t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ep4tsf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>1ep4m5h</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t>How often do you paint your nails?</t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ep4m5h/how_often_do_you_paint_your_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>1ep4fcw</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t>VoyageHues - Watermelon. It's a thermal. I am obsessed! &lt;3</t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c43j4u79rwhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>1ep4dlq</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t>Accidentally matched my glasses!</t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ep4dlq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>1ep48rb</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t>i think this is the best nail idea i’ve ever had 😩</t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/a8uuot9zpwhd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>1ep3pwi</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sally Hansen in dollar tree. </t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ep3pwi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>1ep31ud</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>Mismatched summer skittle (pink grapefruit &amp; calamansi &amp; blueberry smoothie, Ethereal)</t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ep31ud</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>1ep316w</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t>Advice for chrome/metallic polishes?</t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ep316w/advice_for_chromemetallic_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>1ep2ye9</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This shade reminds me of a good temperature solder joint </t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jbgwypgefwhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>1ep2mci</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t>If you've been sleeping on Flower Child...wake up 💖💙</t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ep2mci</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>1ep26ly</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tried to go on a Psilocybin trip 🍄 How’d I do? </t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/z7wgxl919whd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>1ep1uvu</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t>💚 Brat 💚</t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ep1uvu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>1ep177k</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t>These remind me of Trolli sour egg candy</t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ep177k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>1ep14c3</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t>Polished for Days Glowstick</t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/T7ysnJw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>1ep0spq</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t xml:space="preserve">chrome powder on lacquer? </t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ep0spq/chrome_powder_on_lacquer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>1ep0r6m</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t>Strongest magnetic wand recs?</t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ep0r6m/strongest_magnetic_wand_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>1eoz20k</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t>Vaporize by Mooncat discontinued :( Any recommendations?</t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eoz20k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>1eoyshz</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t>Can’t find anything on these online anyone try it before?</t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eoyshz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>1eoyn0m</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t>Pompompurin Nails!! &lt;3</t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eoyn0m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>1eoy8er</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t>The perfect intersection of my 2 hobbies ~ nails and books!</t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eoy8er</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>1eox5zh</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t>Orange mix and match</t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eox5zh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>1eowzd4</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t>What are your favorite pruglies?</t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1eowzd4/what_are_your_favorite_pruglies/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="inlineStr">
+        <is>
+          <t>1eowz9m</t>
+        </is>
+      </c>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t>What's your Holy Trinity?</t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2fjgifwd4vhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="inlineStr">
+        <is>
+          <t>1eowxz9</t>
+        </is>
+      </c>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t>So glowwy ✨️</t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eowxz9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="inlineStr">
+        <is>
+          <t>1eowtto</t>
+        </is>
+      </c>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t>Covergirl should bring back NailSlicks :(</t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1eowtto/covergirl_should_bring_back_nailslicks/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="inlineStr">
+        <is>
+          <t>1eowmn2</t>
+        </is>
+      </c>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t>Got engaged wearing pixie party :)</t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eowmn2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="inlineStr">
+        <is>
+          <t>1eowhyt</t>
+        </is>
+      </c>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t>My attempt at a birthstone skittle</t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eowhyt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="inlineStr">
+        <is>
+          <t>1eowfa6</t>
+        </is>
+      </c>
+      <c r="B1270" t="inlineStr">
+        <is>
+          <t>Along for the ride</t>
+        </is>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eowfa6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="inlineStr">
+        <is>
+          <t>1eow279</t>
+        </is>
+      </c>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t xml:space="preserve">my favourite colour </t>
+        </is>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n40sjhlbxuhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="inlineStr">
+        <is>
+          <t>1eov1if</t>
+        </is>
+      </c>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mixed metals </t>
+        </is>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rws7n5phpuhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="inlineStr">
+        <is>
+          <t>1eou61f</t>
+        </is>
+      </c>
+      <c r="B1273" t="inlineStr">
+        <is>
+          <t>Mehndi with nail paint 🤎💜</t>
+        </is>
+      </c>
+      <c r="C1273" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eou61f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" t="inlineStr">
+        <is>
+          <t>1eou4q9</t>
+        </is>
+      </c>
+      <c r="B1274" t="inlineStr">
+        <is>
+          <t>Neon lime green and flakies ✨🍋‍🟩</t>
+        </is>
+      </c>
+      <c r="C1274" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eou4q9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="inlineStr">
+        <is>
+          <t>1eotpqf</t>
+        </is>
+      </c>
+      <c r="B1275" t="inlineStr">
+        <is>
+          <t>🐴 horseshoe magnet 🐴</t>
+        </is>
+      </c>
+      <c r="C1275" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7d1a92queuhd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" t="inlineStr">
+        <is>
+          <t>1eorrdz</t>
+        </is>
+      </c>
+      <c r="B1276" t="inlineStr">
+        <is>
+          <t>Anyone else doing a Project Polish?</t>
+        </is>
+      </c>
+      <c r="C1276" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tgnfat5pxthd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" t="inlineStr">
+        <is>
+          <t>1eorioq</t>
+        </is>
+      </c>
+      <c r="B1277" t="inlineStr">
+        <is>
+          <t>Rainbow Connection (UK online shop) haul</t>
+        </is>
+      </c>
+      <c r="C1277" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eorioq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="inlineStr">
+        <is>
+          <t>1eopfyc</t>
+        </is>
+      </c>
+      <c r="B1278" t="inlineStr">
+        <is>
+          <t>HHC Monthly Megathread</t>
+        </is>
+      </c>
+      <c r="C1278" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1eopfyc/hhc_monthly_megathread/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" t="inlineStr">
+        <is>
+          <t>1eop9bz</t>
+        </is>
+      </c>
+      <c r="B1279" t="inlineStr">
+        <is>
+          <t>The longest they have been in years!</t>
+        </is>
+      </c>
+      <c r="C1279" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ss3scpt66thd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="inlineStr">
+        <is>
+          <t>1epf87i</t>
+        </is>
+      </c>
+      <c r="B1280" t="inlineStr">
+        <is>
+          <t>A cute little cloud and butterfly set done by my favorite Nail Tech!!</t>
+        </is>
+      </c>
+      <c r="C1280" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7r6hwmownzhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="inlineStr">
+        <is>
+          <t>1epaicp</t>
+        </is>
+      </c>
+      <c r="B1281" t="inlineStr">
+        <is>
+          <t>Some fairy sets i did a few months back✨</t>
+        </is>
+      </c>
+      <c r="C1281" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1epaicp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="inlineStr">
+        <is>
+          <t>1ep8rcr</t>
+        </is>
+      </c>
+      <c r="B1282" t="inlineStr">
+        <is>
+          <t>Looking for all the Super Graphic Ultra Modern Girls🛸🪐🩶</t>
+        </is>
+      </c>
+      <c r="C1282" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ep8rcr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="inlineStr">
+        <is>
+          <t>1ep8l1y</t>
+        </is>
+      </c>
+      <c r="B1283" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gel nail remover! </t>
+        </is>
+      </c>
+      <c r="C1283" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1ep8l1y/gel_nail_remover/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="inlineStr">
+        <is>
+          <t>1ep8fgm</t>
+        </is>
+      </c>
+      <c r="B1284" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Among us nails </t>
+        </is>
+      </c>
+      <c r="C1284" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ep8fgm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="inlineStr">
+        <is>
+          <t>1ep7qpu</t>
+        </is>
+      </c>
+      <c r="B1285" t="inlineStr">
+        <is>
+          <t>Custom $uicideboy$ and TØP Sets</t>
+        </is>
+      </c>
+      <c r="C1285" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ep7qpu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="inlineStr">
+        <is>
+          <t>1ep7q3j</t>
+        </is>
+      </c>
+      <c r="B1286" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Koi Fish Nails by me </t>
+        </is>
+      </c>
+      <c r="C1286" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i1z7f1bljxhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="inlineStr">
+        <is>
+          <t>1ep5ncv</t>
+        </is>
+      </c>
+      <c r="B1287" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fairy barbie nails by me :) </t>
+        </is>
+      </c>
+      <c r="C1287" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ep5ncv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" t="inlineStr">
+        <is>
+          <t>1ep5dns</t>
+        </is>
+      </c>
+      <c r="B1288" t="inlineStr">
+        <is>
+          <t>I love this effect! Do you know what it's called?</t>
+        </is>
+      </c>
+      <c r="C1288" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d5uoeqcgzwhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="inlineStr">
+        <is>
+          <t>1ep59i3</t>
+        </is>
+      </c>
+      <c r="B1289" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The set I did on my sister </t>
+        </is>
+      </c>
+      <c r="C1289" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ep59i3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" t="inlineStr">
+        <is>
+          <t>1ep410o</t>
+        </is>
+      </c>
+      <c r="B1290" t="inlineStr">
+        <is>
+          <t>Spidey nails🕸️🕷️❤️🩵</t>
+        </is>
+      </c>
+      <c r="C1290" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/te8juyp8owhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" t="inlineStr">
+        <is>
+          <t>1ep3xta</t>
+        </is>
+      </c>
+      <c r="B1291" t="inlineStr">
+        <is>
+          <t>Hopping on the strawberry trend</t>
+        </is>
+      </c>
+      <c r="C1291" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gawpltxdnwhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="inlineStr">
+        <is>
+          <t>1ep2z3d</t>
+        </is>
+      </c>
+      <c r="B1292" t="inlineStr">
+        <is>
+          <t>Do you like my nails? 🫶🏼</t>
+        </is>
+      </c>
+      <c r="C1292" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q30sgj9kfwhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="inlineStr">
+        <is>
+          <t>1eovdyr</t>
+        </is>
+      </c>
+      <c r="B1293" t="inlineStr">
+        <is>
+          <t>Any Soul Eater fans?🖤</t>
+        </is>
+      </c>
+      <c r="C1293" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/st1dflb4suhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="inlineStr">
+        <is>
+          <t>1eov712</t>
+        </is>
+      </c>
+      <c r="B1294" t="inlineStr">
+        <is>
+          <t>New acrylic nail set🎀🩷</t>
+        </is>
+      </c>
+      <c r="C1294" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3cltofamquhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" t="inlineStr">
+        <is>
+          <t>1eosmba</t>
+        </is>
+      </c>
+      <c r="B1295" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Finished my nails for the $B concert! </t>
+        </is>
+      </c>
+      <c r="C1295" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ruzu7roh5uhd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" t="inlineStr">
+        <is>
+          <t>1eorb8o</t>
+        </is>
+      </c>
+      <c r="B1296" t="inlineStr">
+        <is>
+          <t>Was qchuffed with these until I thought that the flowers look a bit like fried eggs 😂</t>
+        </is>
+      </c>
+      <c r="C1296" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/euzy2jtdtthd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" t="inlineStr">
+        <is>
+          <t>1eopswf</t>
+        </is>
+      </c>
+      <c r="B1297" t="inlineStr">
+        <is>
+          <t>Good nail strip brands suggestions.</t>
+        </is>
+      </c>
+      <c r="C1297" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1eopswf/good_nail_strip_brands_suggestions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" t="inlineStr">
+        <is>
+          <t>1eopp2c</t>
+        </is>
+      </c>
+      <c r="B1298" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hearts </t>
+        </is>
+      </c>
+      <c r="C1298" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eopp2c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" t="inlineStr">
+        <is>
+          <t>1eookf9</t>
+        </is>
+      </c>
+      <c r="B1299" t="inlineStr">
+        <is>
+          <t>I'm obsessed with kawaii nails and you? 💖🥰🙈</t>
+        </is>
+      </c>
+      <c r="C1299" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eookf9</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>